<commit_message>
4/2 Commit before I implement Sulaiman's changes. Most windows completed.
</commit_message>
<xml_diff>
--- a/Accounts.xlsx
+++ b/Accounts.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -79,6 +82,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
4/5 Backend Code Implemented for sign in and homepage
</commit_message>
<xml_diff>
--- a/Accounts.xlsx
+++ b/Accounts.xlsx
@@ -12,12 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>1</t>
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>molinari</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -96,6 +114,48 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed transitions between panes in ClassOverview, finished styling tables, print is fully functional
</commit_message>
<xml_diff>
--- a/Accounts.xlsx
+++ b/Accounts.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -117,6 +120,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>